<commit_message>
Bump to 0.7.0.  Bug fixes for Tickets 9, 12, 14, 16, and 17.  Fixed bug when a JETT formula replacement accidentally matches as a substring to another formula that shouldn't be affected.  Upgraded JETT to use Apache POI 3.10-FINAL and jAgg 0.7.2.  Allow multi-sheet, multi-map mode to have template sheets in any order and they can be non-consecutive in the template and in the template sheet names list.  Added JUnit tests for AttributeEvaluator.  Added cell locations to Exception messages where appropriate.
</commit_message>
<xml_diff>
--- a/jett-core/templates/FormulaTemplate.xlsx
+++ b/jett-core/templates/FormulaTemplate.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Formula Test" sheetId="1" r:id="rId1"/>
     <sheet name="Cloning" sheetId="2" r:id="rId2"/>
     <sheet name="MultiLevel" sheetId="3" r:id="rId3"/>
+    <sheet name="Copy Right" sheetId="4" r:id="rId4"/>
+    <sheet name="ReplaceTest" sheetId="5" r:id="rId5"/>
+    <sheet name="Outside Reference" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
   <si>
     <t>The State of ${california.name}</t>
   </si>
@@ -213,6 +216,45 @@
   </si>
   <si>
     <t>$[COUNTA('Formula Test'!$K$3)]</t>
+  </si>
+  <si>
+    <t>&lt;jt:for start="1" end="10" var="n" copyRight="true"&gt;${n}</t>
+  </si>
+  <si>
+    <t>${2*n}</t>
+  </si>
+  <si>
+    <t>$[SUM(A1+A2)]</t>
+  </si>
+  <si>
+    <t>&lt;/jt:for&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:for start="1" end="10" var="n"&gt;${n}</t>
+  </si>
+  <si>
+    <t>${two}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${primes}" var="x"&gt;${x}</t>
+  </si>
+  <si>
+    <t>$[A1 * B1]</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${morePrimes}" var="y"&gt;${y}</t>
+  </si>
+  <si>
+    <t>$[A1 * B1 * D1]</t>
+  </si>
+  <si>
+    <t>&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Population Different?</t>
+  </si>
+  <si>
+    <t>$[B4 &lt;&gt; H4]</t>
   </si>
 </sst>
 </file>
@@ -715,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -860,6 +902,14 @@
         <v>47</v>
       </c>
       <c r="L4" s="7"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1088,4 +1138,105 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ticket 43 - Fix parsing JETT Formula text out of cell text when bracket characters exist in the formula itself.
</commit_message>
<xml_diff>
--- a/jett-core/templates/FormulaTemplate.xlsx
+++ b/jett-core/templates/FormulaTemplate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>The State of ${california.name}</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>$[B4 &lt;&gt; H4]</t>
+  </si>
+  <si>
+    <t>Bracket Test</t>
+  </si>
+  <si>
+    <t>$[TEXT(39300.625, "[h]")]</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -909,6 +915,14 @@
       </c>
       <c r="C6" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Ticket 58 - Tag Parser now ignores text inside JETT formulas, for the purpose of finding the start of a tag.  Now a '<' character in a JETT formula won't make the TagParser complain about a missing end to a tag.
</commit_message>
<xml_diff>
--- a/jett-core/templates/FormulaTemplate.xlsx
+++ b/jett-core/templates/FormulaTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17115" windowHeight="10230" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="17115" windowHeight="10230"/>
   </bookViews>
   <sheets>
     <sheet name="Formula Test" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Outside Reference" sheetId="6" r:id="rId6"/>
     <sheet name="MultiLevel2" sheetId="7" r:id="rId7"/>
     <sheet name="Grid" sheetId="8" r:id="rId8"/>
+    <sheet name="TagParseInFormula" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
   <si>
     <t>The State of ${california.name}</t>
   </si>
@@ -353,6 +354,15 @@
   </si>
   <si>
     <t>&lt;jt:forEach items="${dates}" var="date" copyRight="true" indexVar="i"&gt;&lt;jt:formula text="SUM(OFFSET(B2, 0, ${i}, ${regions.size()}, 1))"/&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="true"&gt;</t>
+  </si>
+  <si>
+    <t>$[MIN((N2&gt;=$P$1)*(N2&lt;$R$1))]</t>
+  </si>
+  <si>
+    <t>&lt;/jt:if&gt;</t>
   </si>
 </sst>
 </file>
@@ -537,6 +547,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -554,15 +573,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -888,22 +898,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="15"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
     </row>
     <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1052,14 +1062,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1146,14 +1156,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
       <c r="H1" t="s">
         <v>44</v>
       </c>
@@ -1368,35 +1378,35 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1404,30 +1414,30 @@
       <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="14" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1437,34 +1447,34 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="14" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1478,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1486,13 +1496,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1503,7 +1513,7 @@
       <c r="B2" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D2" t="s">
@@ -1511,18 +1521,46 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R15" s="20"/>
+      <c r="R15" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ticket 79 - Fix implicit sheet cloning case when the number of items in the collection is 1. Ticket 81 - Create the jt:pageBreak tag. Ticket 82 - Update cell reference in formula even if no space precedes it.
</commit_message>
<xml_diff>
--- a/jett-core/templates/FormulaTemplate.xlsx
+++ b/jett-core/templates/FormulaTemplate.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\files\subv\jett\jett-core\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="17115" windowHeight="10230"/>
+    <workbookView xWindow="120" yWindow="36" windowWidth="17112" windowHeight="10236"/>
   </bookViews>
   <sheets>
     <sheet name="Formula Test" sheetId="1" r:id="rId1"/>
@@ -16,13 +21,14 @@
     <sheet name="MultiLevel2" sheetId="7" r:id="rId7"/>
     <sheet name="Grid" sheetId="8" r:id="rId8"/>
     <sheet name="TagParseInFormula" sheetId="9" r:id="rId9"/>
+    <sheet name="NoSpaceAfterParen" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="114">
   <si>
     <t>The State of ${california.name}</t>
   </si>
@@ -363,6 +369,30 @@
   </si>
   <si>
     <t>&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>&lt;jt:for start="1" end="10" var="x"&gt;${x}</t>
+  </si>
+  <si>
+    <t>${x+1}</t>
+  </si>
+  <si>
+    <t>${x+2}</t>
+  </si>
+  <si>
+    <t>$[A2-(IF(B2="-",0,B2)+C2)]</t>
   </si>
 </sst>
 </file>
@@ -532,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -574,6 +604,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,6 +616,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -631,7 +667,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -666,7 +702,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -881,23 +917,23 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -915,7 +951,7 @@
       <c r="K1" s="19"/>
       <c r="L1" s="20"/>
     </row>
-    <row r="2" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -953,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -991,7 +1027,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -1021,7 +1057,7 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1029,7 +1065,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -1044,6 +1080,51 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1055,13 +1136,13 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1152,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="24"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1091,7 +1172,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1111,7 +1192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -1148,14 +1229,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>50</v>
       </c>
@@ -1171,7 +1252,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
@@ -1197,7 +1278,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>51</v>
       </c>
@@ -1217,7 +1298,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>42</v>
       </c>
@@ -1237,7 +1318,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -1270,28 +1351,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1307,24 +1386,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1342,9 +1421,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1373,17 +1452,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>73</v>
       </c>
@@ -1397,7 +1478,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>74</v>
       </c>
@@ -1405,12 +1486,12 @@
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1427,7 +1508,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>83</v>
       </c>
@@ -1441,12 +1522,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>87</v>
       </c>
@@ -1463,8 +1544,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>91</v>
       </c>
@@ -1490,12 +1571,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>98</v>
       </c>
@@ -1506,7 +1587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
@@ -1520,7 +1601,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
@@ -1531,7 +1612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R15" s="14"/>
     </row>
   </sheetData>
@@ -1543,21 +1624,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>

</xml_diff>